<commit_message>
add new files and update some
</commit_message>
<xml_diff>
--- a/hotel-management/data/excel/booking.xlsx
+++ b/hotel-management/data/excel/booking.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking information of The Doe" r:id="rId3" sheetId="1"/>
+    <sheet name="Booking information of wutemey" r:id="rId4" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Booking ID</t>
   </si>
@@ -38,46 +38,25 @@
     <t>Pricing</t>
   </si>
   <si>
-    <t>03a0becd60e25bf92a7576180ac9d539</t>
+    <t>5778f857c4d839489044db6a62007906</t>
   </si>
   <si>
-    <t>Stiedemann-Ankunding</t>
+    <t>Olson-Roberts</t>
   </si>
   <si>
-    <t>74 Farmco Street</t>
+    <t>8 Hudson Center</t>
   </si>
   <si>
-    <t>Seaberry</t>
+    <t>Wildrye</t>
   </si>
   <si>
-    <t>26/02/2024</t>
+    <t>01/01/2020</t>
   </si>
   <si>
-    <t>26/03/2024</t>
+    <t>02/02/2020</t>
   </si>
   <si>
-    <t>514214</t>
-  </si>
-  <si>
-    <t>de9a4f415b0784cdd268c6aee348e708</t>
-  </si>
-  <si>
-    <t>"Senger</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Harris and Parisian"</t>
-  </si>
-  <si>
-    <t>Madagascar Flatsedge</t>
-  </si>
-  <si>
-    <t>01/02/2024</t>
-  </si>
-  <si>
-    <t>04/02/2024</t>
-  </si>
-  <si>
-    <t>449223</t>
+    <t>52901</t>
   </si>
 </sst>
 </file>
@@ -122,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -168,7 +147,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -180,32 +159,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>